<commit_message>
practiced merge sort algorithm
</commit_message>
<xml_diff>
--- a/dsa_log.xlsx
+++ b/dsa_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richa/Library/CloudStorage/OneDrive-Personal/Documents/SCHOOL/CODING/DSA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d34f119de7acea51/Documents/SCHOOL/CODING/DSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A730C13-FF80-2340-9520-3A3582011BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B01EAFFF-C515-FE44-B1CA-72A77FC378FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="68800" windowHeight="28800" xr2:uid="{BEDA4785-54A3-8F4E-898D-AF93E9363723}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="224">
   <si>
     <t>easy</t>
   </si>
@@ -179,12 +179,6 @@
     <t>convert string, create a reversed temp string then compare with original</t>
   </si>
   <si>
-    <t>palindrome number</t>
-  </si>
-  <si>
-    <t>create temp reversed number compare with original number</t>
-  </si>
-  <si>
     <t>palindrome linked list</t>
   </si>
   <si>
@@ -705,13 +699,22 @@
   </si>
   <si>
     <t>check for the sign, convert to string, reverse string, then convert to int. check for int overflow. Reassign sign if necessary`</t>
+  </si>
+  <si>
+    <t>Palindrome Number</t>
+  </si>
+  <si>
+    <t>negatives can never be palindrome Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge sort </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -746,6 +749,16 @@
     <font>
       <sz val="12"/>
       <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -881,7 +894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -972,6 +985,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1328,10 +1357,14 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6374C534-ADCB-2B48-8495-3E0235A90001}" name="Table2" displayName="Table2" ref="G9:L110" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G10:L110">
-    <sortCondition ref="K9:K110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6374C534-ADCB-2B48-8495-3E0235A90001}" name="Table2" displayName="Table2" ref="G9:L111" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G10:L111">
+    <sortCondition ref="K10:K111"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{EA5305E0-6338-0540-8106-3C232FACFE3A}" name="QUESTION" dataDxfId="5"/>
@@ -1664,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398B4FC1-FB0D-D846-BD25-3C3153F03FF8}">
   <dimension ref="A9:L112"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F39" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="J79" sqref="J79"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F86" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
+      <selection activeCell="G110" sqref="G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1685,22 +1718,22 @@
   <sheetData>
     <row r="9" spans="7:12" s="2" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G9" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="L9" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="10" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
@@ -1805,13 +1838,13 @@
     </row>
     <row r="15" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G15" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J15" s="9">
         <v>0</v>
@@ -1851,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J17" s="9">
         <v>0</v>
@@ -1865,13 +1898,13 @@
     </row>
     <row r="18" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G18" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J18" s="9">
         <v>0</v>
@@ -1905,13 +1938,13 @@
     </row>
     <row r="20" spans="7:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G20" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J20" s="9">
         <v>0</v>
@@ -1920,7 +1953,7 @@
         <v>12</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="7:12" x14ac:dyDescent="0.2">
@@ -1951,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J22" s="9">
         <v>0</v>
@@ -1985,13 +2018,13 @@
     </row>
     <row r="24" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G24" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J24" s="9">
         <v>0</v>
@@ -2025,13 +2058,13 @@
     </row>
     <row r="26" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G26" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J26" s="9">
         <v>0</v>
@@ -2065,13 +2098,13 @@
     </row>
     <row r="28" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G28" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J28" s="9">
         <v>0</v>
@@ -2080,12 +2113,12 @@
         <v>12</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G29" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>0</v>
@@ -2105,13 +2138,13 @@
     </row>
     <row r="30" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G30" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H30" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J30" s="9">
         <v>0</v>
@@ -2120,18 +2153,18 @@
         <v>12</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G31" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H31" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J31" s="9">
         <v>0</v>
@@ -2140,7 +2173,7 @@
         <v>12</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="7:12" x14ac:dyDescent="0.2">
@@ -2165,13 +2198,13 @@
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G33" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J33" s="9">
         <v>0</v>
@@ -2180,18 +2213,18 @@
         <v>12</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G34" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J34" s="9">
         <v>0</v>
@@ -2205,13 +2238,13 @@
     </row>
     <row r="35" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G35" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H35" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J35" s="9">
         <v>0</v>
@@ -2225,13 +2258,13 @@
     </row>
     <row r="36" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G36" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J36" s="9">
         <v>0</v>
@@ -2240,18 +2273,18 @@
         <v>12</v>
       </c>
       <c r="L36" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G37" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H37" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J37" s="9">
         <v>0</v>
@@ -2285,13 +2318,13 @@
     </row>
     <row r="39" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G39" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I39" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="J39" s="9">
         <v>0</v>
@@ -2300,18 +2333,18 @@
         <v>12</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G40" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H40" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J40" s="9">
         <v>0</v>
@@ -2325,13 +2358,13 @@
     </row>
     <row r="41" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G41" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H41" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J41" s="9">
         <v>0</v>
@@ -2345,13 +2378,13 @@
     </row>
     <row r="42" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G42" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J42" s="9">
         <v>0</v>
@@ -2365,13 +2398,13 @@
     </row>
     <row r="43" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G43" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H43" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J43" s="9">
         <v>0</v>
@@ -2385,13 +2418,13 @@
     </row>
     <row r="44" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G44" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H44" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J44" s="9">
         <v>0</v>
@@ -2405,13 +2438,13 @@
     </row>
     <row r="45" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G45" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H45" s="21" t="s">
         <v>30</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J45" s="23">
         <v>0</v>
@@ -2425,13 +2458,13 @@
     </row>
     <row r="46" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G46" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H46" s="21" t="s">
         <v>30</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J46" s="23">
         <v>0</v>
@@ -2445,13 +2478,13 @@
     </row>
     <row r="47" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G47" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H47" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J47" s="9">
         <v>0</v>
@@ -2471,13 +2504,13 @@
         <v>0</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J48" s="23">
         <v>0</v>
       </c>
       <c r="K48" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L48" s="24" t="s">
         <v>9</v>
@@ -2485,22 +2518,22 @@
     </row>
     <row r="49" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G49" s="20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H49" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J49" s="23">
         <v>0</v>
       </c>
       <c r="K49" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L49" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="7:12" x14ac:dyDescent="0.2">
@@ -2517,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>9</v>
@@ -2537,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>9</v>
@@ -2557,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>9</v>
@@ -2565,19 +2598,19 @@
     </row>
     <row r="53" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G53" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H53" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J53" s="9">
         <v>0</v>
       </c>
       <c r="K53" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L53" s="10" t="s">
         <v>9</v>
@@ -2585,19 +2618,19 @@
     </row>
     <row r="54" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G54" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H54" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I54" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J54" s="9">
+        <v>0</v>
+      </c>
+      <c r="K54" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="J54" s="9">
-        <v>0</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>137</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>9</v>
@@ -2605,7 +2638,7 @@
     </row>
     <row r="55" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G55" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>0</v>
@@ -2617,10 +2650,10 @@
         <v>0</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="7:12" x14ac:dyDescent="0.2">
@@ -2637,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>9</v>
@@ -2657,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>9</v>
@@ -2665,39 +2698,39 @@
     </row>
     <row r="58" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G58" s="20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H58" s="22" t="s">
         <v>30</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J58" s="23">
         <v>0</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L58" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G59" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H59" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J59" s="9">
         <v>0</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L59" s="10" t="s">
         <v>9</v>
@@ -2705,39 +2738,39 @@
     </row>
     <row r="60" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G60" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J60" s="9">
         <v>0</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G61" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J61" s="9">
         <v>0</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>9</v>
@@ -2745,19 +2778,19 @@
     </row>
     <row r="62" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G62" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J62" s="9">
         <v>0</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>9</v>
@@ -2765,39 +2798,39 @@
     </row>
     <row r="63" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G63" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H63" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J63" s="9">
         <v>0</v>
       </c>
       <c r="K63" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L63" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G64" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H64" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J64" s="9">
         <v>0</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>9</v>
@@ -2805,19 +2838,19 @@
     </row>
     <row r="65" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G65" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J65" s="9">
         <v>0</v>
       </c>
       <c r="K65" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>9</v>
@@ -2825,19 +2858,19 @@
     </row>
     <row r="66" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G66" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I66" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J66" s="14">
         <v>0</v>
       </c>
       <c r="K66" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L66" s="15" t="s">
         <v>9</v>
@@ -2845,199 +2878,199 @@
     </row>
     <row r="67" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G67" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I67" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J67" s="14">
         <v>0</v>
       </c>
       <c r="K67" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L67" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G68" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="J68" s="14">
+        <v>0</v>
+      </c>
+      <c r="K68" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="H68" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I68" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="J68" s="14">
-        <v>0</v>
-      </c>
-      <c r="K68" s="14" t="s">
-        <v>204</v>
-      </c>
       <c r="L68" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G69" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H69" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I69" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J69" s="14">
         <v>0</v>
       </c>
       <c r="K69" s="14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L69" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="70" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G70" s="26" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H70" s="27" t="s">
         <v>0</v>
       </c>
       <c r="I70" s="28" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J70" s="29">
         <v>0</v>
       </c>
       <c r="K70" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L70" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G71" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H71" s="27" t="s">
         <v>0</v>
       </c>
       <c r="I71" s="28" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J71" s="29">
         <v>0</v>
       </c>
       <c r="K71" s="29" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L71" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G72" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H72" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J72" s="14">
         <v>0</v>
       </c>
       <c r="K72" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L72" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G73" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H73" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I73" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="J73" s="14">
+        <v>0</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L73" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="H73" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I73" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J73" s="14">
-        <v>0</v>
-      </c>
-      <c r="K73" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L73" s="15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="74" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G74" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H74" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I74" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J74" s="14">
         <v>0</v>
       </c>
       <c r="K74" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L74" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G75" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H75" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I75" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J75" s="14">
         <v>0</v>
       </c>
       <c r="K75" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L75" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G76" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H76" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I76" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J76" s="14">
         <v>0</v>
       </c>
       <c r="K76" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L76" s="15" t="s">
         <v>9</v>
@@ -3045,19 +3078,19 @@
     </row>
     <row r="77" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G77" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H77" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I77" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J77" s="14">
+        <v>0</v>
+      </c>
+      <c r="K77" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="J77" s="14">
-        <v>0</v>
-      </c>
-      <c r="K77" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="L77" s="15" t="s">
         <v>9</v>
@@ -3065,142 +3098,142 @@
     </row>
     <row r="78" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G78" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H78" s="12" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I78" s="13" t="s">
-        <v>48</v>
+        <v>220</v>
       </c>
       <c r="J78" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L78" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G79" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H79" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I79" s="13" t="s">
+      <c r="G79" s="26" t="s">
+        <v>218</v>
+      </c>
+      <c r="H79" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I79" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="J79" s="29">
+        <v>0</v>
+      </c>
+      <c r="K79" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="L79" s="30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G80" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="H80" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="I80" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="J79" s="14">
-        <v>1</v>
-      </c>
-      <c r="K79" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="L79" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G80" s="11" t="s">
+      <c r="J80" s="35">
+        <v>0</v>
+      </c>
+      <c r="K80" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="L80" s="36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G81" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="J81" s="14">
+        <v>0</v>
+      </c>
+      <c r="K81" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H80" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I80" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="J80" s="14">
-        <v>0</v>
-      </c>
-      <c r="K80" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="L80" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G81" s="26" t="s">
+      <c r="L81" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G82" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="H82" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I82" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="J82" s="29">
+        <v>0</v>
+      </c>
+      <c r="K82" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="H81" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="I81" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="J81" s="29">
-        <v>0</v>
-      </c>
-      <c r="K81" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="L81" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G82" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H82" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I82" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="J82" s="14">
-        <v>0</v>
-      </c>
-      <c r="K82" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="L82" s="15" t="s">
-        <v>65</v>
+      <c r="L82" s="30" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G83" s="11" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="H83" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
       <c r="J83" s="14">
         <v>0</v>
       </c>
       <c r="K83" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L83" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G84" s="11" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="H84" s="12" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="J84" s="14">
         <v>0</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L84" s="15" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="7:12" x14ac:dyDescent="0.2">
@@ -3208,136 +3241,136 @@
         <v>165</v>
       </c>
       <c r="H85" s="12" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="I85" s="13" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="J85" s="14">
         <v>0</v>
       </c>
       <c r="K85" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L85" s="15" t="s">
-        <v>169</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G86" s="11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="H86" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="J86" s="14">
         <v>0</v>
       </c>
       <c r="K86" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L86" s="15" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G87" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H87" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J87" s="14">
         <v>0</v>
       </c>
       <c r="K87" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G88" s="11" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="H88" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I88" s="13" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="J88" s="14">
         <v>0</v>
       </c>
       <c r="K88" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L88" s="15" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G89" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="H89" s="27" t="s">
+      <c r="G89" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H89" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I89" s="28" t="s">
-        <v>175</v>
-      </c>
-      <c r="J89" s="29">
-        <v>0</v>
-      </c>
-      <c r="K89" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="L89" s="30" t="s">
+      <c r="I89" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="J89" s="14">
+        <v>0</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="L89" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="90" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G90" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="H90" s="12" t="s">
+      <c r="G90" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H90" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="I90" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="J90" s="14">
-        <v>0</v>
-      </c>
-      <c r="K90" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="L90" s="15" t="s">
+      <c r="I90" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="J90" s="29">
+        <v>0</v>
+      </c>
+      <c r="K90" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L90" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="91" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G91" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H91" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I91" s="13" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J91" s="14">
         <v>0</v>
       </c>
       <c r="K91" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L91" s="15" t="s">
         <v>9</v>
@@ -3345,19 +3378,19 @@
     </row>
     <row r="92" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G92" s="11" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H92" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="J92" s="14">
         <v>0</v>
       </c>
       <c r="K92" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L92" s="15" t="s">
         <v>9</v>
@@ -3365,19 +3398,19 @@
     </row>
     <row r="93" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G93" s="11" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H93" s="12" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J93" s="14">
         <v>0</v>
       </c>
       <c r="K93" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L93" s="15" t="s">
         <v>9</v>
@@ -3385,119 +3418,119 @@
     </row>
     <row r="94" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G94" s="11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="J94" s="14">
         <v>0</v>
       </c>
       <c r="K94" s="14" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
       <c r="L94" s="15" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G95" s="11" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H95" s="12" t="s">
         <v>0</v>
       </c>
       <c r="I95" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="J95" s="14">
+        <v>0</v>
+      </c>
+      <c r="K95" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="J95" s="14">
-        <v>0</v>
-      </c>
-      <c r="K95" s="14" t="s">
-        <v>190</v>
-      </c>
       <c r="L95" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="96" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G96" s="11" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="H96" s="12" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I96" s="13" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="J96" s="14">
         <v>0</v>
       </c>
       <c r="K96" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L96" s="15" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="97" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G97" s="11" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H97" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I97" s="13" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J97" s="14">
         <v>0</v>
       </c>
       <c r="K97" s="14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L97" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="98" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G98" s="26" t="s">
-        <v>211</v>
-      </c>
-      <c r="H98" s="27" t="s">
+      <c r="G98" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="H98" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I98" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="J98" s="29">
-        <v>0</v>
-      </c>
-      <c r="K98" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="L98" s="30" t="s">
+      <c r="I98" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="J98" s="14">
+        <v>0</v>
+      </c>
+      <c r="K98" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="L98" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="99" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G99" s="26" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="H99" s="27" t="s">
-        <v>157</v>
+        <v>30</v>
       </c>
       <c r="I99" s="28" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="J99" s="29">
         <v>0</v>
       </c>
       <c r="K99" s="29" t="s">
-        <v>31</v>
+        <v>211</v>
       </c>
       <c r="L99" s="30" t="s">
         <v>9</v>
@@ -3505,13 +3538,13 @@
     </row>
     <row r="100" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G100" s="26" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="H100" s="27" t="s">
-        <v>30</v>
+        <v>155</v>
       </c>
       <c r="I100" s="28" t="s">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="J100" s="29">
         <v>0</v>
@@ -3524,34 +3557,34 @@
       </c>
     </row>
     <row r="101" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G101" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H101" s="12" t="s">
+      <c r="G101" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="H101" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="I101" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J101" s="14">
-        <v>0</v>
-      </c>
-      <c r="K101" s="14" t="s">
+      <c r="I101" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="J101" s="29">
+        <v>0</v>
+      </c>
+      <c r="K101" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="L101" s="15" t="s">
+      <c r="L101" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="102" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G102" s="11" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="H102" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I102" s="13" t="s">
-        <v>155</v>
+        <v>60</v>
       </c>
       <c r="J102" s="14">
         <v>0</v>
@@ -3560,136 +3593,148 @@
         <v>31</v>
       </c>
       <c r="L102" s="15" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G103" s="26" t="s">
+      <c r="G103" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H103" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I103" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="J103" s="14">
+        <v>0</v>
+      </c>
+      <c r="K103" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L103" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G104" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H104" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I104" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="H103" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="I103" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="J103" s="29">
-        <v>0</v>
-      </c>
-      <c r="K103" s="29" t="s">
+      <c r="J104" s="29">
+        <v>0</v>
+      </c>
+      <c r="K104" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="L103" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G104" s="11" t="s">
+      <c r="L104" s="30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G105" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H104" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="I104" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="J104" s="14">
-        <v>0</v>
-      </c>
-      <c r="K104" s="14" t="s">
+      <c r="H105" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I105" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J105" s="14">
+        <v>0</v>
+      </c>
+      <c r="K105" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="L104" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="105" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="G105" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="H105" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="I105" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="J105" s="29">
-        <v>2</v>
-      </c>
-      <c r="K105" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="L105" s="30" t="s">
-        <v>65</v>
+      <c r="L105" s="15" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="7:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G106" s="26" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="H106" s="27" t="s">
         <v>0</v>
       </c>
       <c r="I106" s="28" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J106" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K106" s="29" t="s">
         <v>31</v>
       </c>
       <c r="L106" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="107" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G107" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H107" s="27" t="s">
         <v>0</v>
       </c>
       <c r="I107" s="28" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J107" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K107" s="29" t="s">
         <v>31</v>
       </c>
       <c r="L107" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="108" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G108" s="26" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H108" s="27" t="s">
         <v>0</v>
       </c>
       <c r="I108" s="28" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="J108" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K108" s="29" t="s">
-        <v>189</v>
+        <v>31</v>
       </c>
       <c r="L108" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="109" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G109" s="26"/>
-      <c r="H109" s="27"/>
-      <c r="I109" s="28"/>
-      <c r="J109" s="29"/>
-      <c r="K109" s="29"/>
-      <c r="L109" s="30"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="7:12" s="37" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G109" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="H109" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I109" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J109" s="14">
+        <v>0</v>
+      </c>
+      <c r="K109" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="L109" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="110" spans="7:12" x14ac:dyDescent="0.2">
       <c r="G110" s="11"/>
@@ -3698,6 +3743,14 @@
       <c r="J110" s="14"/>
       <c r="K110" s="14"/>
       <c r="L110" s="15"/>
+    </row>
+    <row r="111" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G111" s="11"/>
+      <c r="H111" s="12"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="14"/>
+      <c r="K111" s="14"/>
+      <c r="L111" s="15"/>
     </row>
     <row r="112" spans="7:12" x14ac:dyDescent="0.2">
       <c r="J112" s="31"/>

</xml_diff>